<commit_message>
Update to GAS hierarchy
</commit_message>
<xml_diff>
--- a/data/KAHI_gas.xlsx
+++ b/data/KAHI_gas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE52C4C2-B43C-374B-9282-6D304D9369AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61A143C-8280-6743-9F5F-A77535CDCC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15800" xr2:uid="{D4CC0A2D-E72B-AB45-9E7A-41F2361D5FC0}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -408,16 +408,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,44 +425,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GAS scale update 2
</commit_message>
<xml_diff>
--- a/data/KAHI_gas.xlsx
+++ b/data/KAHI_gas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28864E6-39BA-A54A-BD6D-8527CEFC99A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA2B4FE-E447-9748-8D55-A8699D6F840F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15800" xr2:uid="{D4CC0A2D-E72B-AB45-9E7A-41F2361D5FC0}"/>
   </bookViews>
@@ -56,19 +56,19 @@
     <t>Decline</t>
   </si>
   <si>
-    <t>35 to 45 minutes</t>
-  </si>
-  <si>
-    <t>25 to 35 minutes</t>
-  </si>
-  <si>
-    <t>15 to 25 minutes</t>
-  </si>
-  <si>
-    <t>5 to 15 minutes</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 to 5 minutes </t>
+  </si>
+  <si>
+    <t>6 to 15 minutes</t>
+  </si>
+  <si>
+    <t>16 to 25 minutes</t>
+  </si>
+  <si>
+    <t>26 to 35 minutes</t>
+  </si>
+  <si>
+    <t>36 to 45 minutes</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -470,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>